<commit_message>
Added 10x scRNAseq 1m neurons dataset. Added 10x xenium mouse pup dataset. Updated xenium mouse brain dataset.
</commit_message>
<xml_diff>
--- a/datasets/10x_1M_neurons.xlsx
+++ b/datasets/10x_1M_neurons.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t xml:space="preserve">sample</t>
   </si>
@@ -55,9 +55,6 @@
     <t xml:space="preserve">neurons</t>
   </si>
   <si>
-    <t xml:space="preserve">neurons_1M</t>
-  </si>
-  <si>
     <t xml:space="preserve">10x</t>
   </si>
   <si>
@@ -67,7 +64,16 @@
     <t xml:space="preserve">datasets/10x_1M_neurons/filtered_feature_bc_matrix.h5</t>
   </si>
   <si>
+    <t xml:space="preserve">datasets/10x_1M_neurons/metrics_summary.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datasets/10x_1M_neurons/analysis/kmeans/10_clusters/clusters.csv</t>
+  </si>
+  <si>
     <t xml:space="preserve">ENSEMBL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
   </si>
 </sst>
 </file>
@@ -167,10 +173,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.56"/>
   </cols>
@@ -212,19 +218,28 @@
         <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="I2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>